<commit_message>
Récupération du fichier projet
</commit_message>
<xml_diff>
--- a/OPEN_sujet1_application/Base_de_données.xlsx
+++ b/OPEN_sujet1_application/Base_de_données.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,12 +375,72 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>lat</t>
+          <t>lat...4</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>long</t>
+          <t>long...5</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>lat...6</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>long...7</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>lat...8</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>long...9</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>lat...10</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>long...11</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>lat...12</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>long...13</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>lat...14</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>long...15</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>lat...16</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>long...17</t>
         </is>
       </c>
     </row>
@@ -406,6 +466,42 @@
       <c r="E2">
         <v>2.302215602227763</v>
       </c>
+      <c r="F2">
+        <v>48.86614866335567</v>
+      </c>
+      <c r="G2">
+        <v>2.31900834175702</v>
+      </c>
+      <c r="H2">
+        <v>48.86614866335567</v>
+      </c>
+      <c r="I2">
+        <v>2.31900834175702</v>
+      </c>
+      <c r="J2">
+        <v>48.86614866335567</v>
+      </c>
+      <c r="K2">
+        <v>2.31900834175702</v>
+      </c>
+      <c r="L2">
+        <v>48.87149735714665</v>
+      </c>
+      <c r="M2">
+        <v>2.302215602227763</v>
+      </c>
+      <c r="N2">
+        <v>48.87149735714665</v>
+      </c>
+      <c r="O2">
+        <v>2.302215602227763</v>
+      </c>
+      <c r="P2">
+        <v>48.86833055200977</v>
+      </c>
+      <c r="Q2">
+        <v>2.312151995261002</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -429,6 +525,42 @@
       <c r="E3">
         <v>2.3604077</v>
       </c>
+      <c r="F3">
+        <v>48.8554814</v>
+      </c>
+      <c r="G3">
+        <v>2.3604077</v>
+      </c>
+      <c r="H3">
+        <v>48.8554814</v>
+      </c>
+      <c r="I3">
+        <v>2.3604077</v>
+      </c>
+      <c r="J3">
+        <v>48.8554814</v>
+      </c>
+      <c r="K3">
+        <v>2.3604077</v>
+      </c>
+      <c r="L3">
+        <v>48.8554814</v>
+      </c>
+      <c r="M3">
+        <v>2.3604077</v>
+      </c>
+      <c r="N3">
+        <v>48.8554814</v>
+      </c>
+      <c r="O3">
+        <v>2.3604077</v>
+      </c>
+      <c r="P3">
+        <v>48.8554814</v>
+      </c>
+      <c r="Q3">
+        <v>2.3604077</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -452,6 +584,42 @@
       <c r="E4">
         <v>4.8309221</v>
       </c>
+      <c r="F4">
+        <v>45.7588923</v>
+      </c>
+      <c r="G4">
+        <v>4.8309221</v>
+      </c>
+      <c r="H4">
+        <v>45.7588923</v>
+      </c>
+      <c r="I4">
+        <v>4.8309221</v>
+      </c>
+      <c r="J4">
+        <v>45.7588923</v>
+      </c>
+      <c r="K4">
+        <v>4.8309221</v>
+      </c>
+      <c r="L4">
+        <v>45.7588923</v>
+      </c>
+      <c r="M4">
+        <v>4.8309221</v>
+      </c>
+      <c r="N4">
+        <v>45.7588923</v>
+      </c>
+      <c r="O4">
+        <v>4.8309221</v>
+      </c>
+      <c r="P4">
+        <v>45.7588923</v>
+      </c>
+      <c r="Q4">
+        <v>4.8309221</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -473,6 +641,42 @@
         <v>45.7640318</v>
       </c>
       <c r="E5">
+        <v>4.8356904</v>
+      </c>
+      <c r="F5">
+        <v>45.7640318</v>
+      </c>
+      <c r="G5">
+        <v>4.8356904</v>
+      </c>
+      <c r="H5">
+        <v>45.7640318</v>
+      </c>
+      <c r="I5">
+        <v>4.8356904</v>
+      </c>
+      <c r="J5">
+        <v>45.7640318</v>
+      </c>
+      <c r="K5">
+        <v>4.8356904</v>
+      </c>
+      <c r="L5">
+        <v>45.7640318</v>
+      </c>
+      <c r="M5">
+        <v>4.8356904</v>
+      </c>
+      <c r="N5">
+        <v>45.7640318</v>
+      </c>
+      <c r="O5">
+        <v>4.8356904</v>
+      </c>
+      <c r="P5">
+        <v>45.7640318</v>
+      </c>
+      <c r="Q5">
         <v>4.8356904</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrections avec code qui fonctionne
</commit_message>
<xml_diff>
--- a/OPEN_sujet1_application/Base_de_données.xlsx
+++ b/OPEN_sujet1_application/Base_de_données.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -400,6 +400,12 @@
           <t>1 avenue des Champs-Elysées, 75008 Paris</t>
         </is>
       </c>
+      <c r="D2">
+        <v>48.86614866335567</v>
+      </c>
+      <c r="E2">
+        <v>2.31900834175702</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -417,6 +423,12 @@
           <t>10 Rue de Rivoli, 75004 Paris</t>
         </is>
       </c>
+      <c r="D3">
+        <v>48.8554814</v>
+      </c>
+      <c r="E3">
+        <v>2.3604077</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -434,6 +446,12 @@
           <t>1 place Bellecour, 69002 Lyon</t>
         </is>
       </c>
+      <c r="D4">
+        <v>45.7588923</v>
+      </c>
+      <c r="E4">
+        <v>4.8309221</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -450,6 +468,35 @@
         <is>
           <t>18 Rue de la République, 69001 Lyon</t>
         </is>
+      </c>
+      <c r="D5">
+        <v>45.7640318</v>
+      </c>
+      <c r="E5">
+        <v>4.8356904</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>HATIER</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Cléo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Promenade des Anglais, 06000 Nice</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>43.6859892</v>
+      </c>
+      <c r="E6">
+        <v>7.237476542487647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>